<commit_message>
add select all option
</commit_message>
<xml_diff>
--- a/tfidf_matrix.xlsx
+++ b/tfidf_matrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,49 +515,49 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.09820019979447743</v>
+        <v>0.9853284724047701</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1160547815752915</v>
+        <v>0.1342617650160634</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01278435406533429</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3928007991779097</v>
+        <v>0.02048060822278933</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1167338560540523</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.008927290890407039</v>
+        <v>0.004551246271730962</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01510129091211827</v>
+        <v>0.002275623135865481</v>
       </c>
       <c r="J2" t="n">
-        <v>0.232109563150583</v>
+        <v>0.03868559330971318</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6606195258901209</v>
+        <v>0.06144182466836799</v>
       </c>
       <c r="L2" t="n">
-        <v>0.03570916356162816</v>
+        <v>0.006826869407596443</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0.01278435406533429</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0.5624193260956435</v>
+        <v>0.02226731011084226</v>
       </c>
       <c r="P2" t="n">
-        <v>0.02122433746437315</v>
+        <v>0.06958534409638206</v>
       </c>
     </row>
     <row r="3">
@@ -565,49 +565,49 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.1077132271348133</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1101410130563839</v>
+        <v>0.1320939316800721</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3154555453190162</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.195499508706635</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1101410130563839</v>
+        <v>0.6604696584003606</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.1995708967262472</v>
       </c>
       <c r="H3" t="n">
-        <v>0.05507050652819195</v>
+        <v>0.1761252422400962</v>
       </c>
       <c r="I3" t="n">
-        <v>0.04657828169649891</v>
+        <v>0.04403131056002405</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1101410130563839</v>
+        <v>0.08806262112004809</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8811281044510713</v>
+        <v>0.6604696584003606</v>
       </c>
       <c r="L3" t="n">
-        <v>0.05507050652819195</v>
+        <v>0.04403131056002405</v>
       </c>
       <c r="M3" t="n">
-        <v>0.195499508706635</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>0.06652363224208238</v>
       </c>
       <c r="O3" t="n">
-        <v>0.05507050652819195</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>0.1077132271348133</v>
       </c>
     </row>
     <row r="4">
@@ -615,49 +615,49 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1014173122144779</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1774802963753362</v>
+        <v>0.108722157306214</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.3285204422586898</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.2083432623952618</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1267716402680973</v>
+        <v>0.108722157306214</v>
       </c>
       <c r="G4" t="n">
-        <v>0.03013953624893626</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1267716402680973</v>
+        <v>0.05436107865310699</v>
       </c>
       <c r="I4" t="n">
-        <v>0.02144452827399307</v>
+        <v>0.05436107865310699</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2028346244289557</v>
+        <v>0.108722157306214</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9381101379839202</v>
+        <v>0.8697772584497118</v>
       </c>
       <c r="L4" t="n">
-        <v>0.02535432805361947</v>
+        <v>0.05436107865310699</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>0.2083432623952618</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0363087425855494</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>0.02535432805361947</v>
+        <v>0.06649140279703235</v>
       </c>
       <c r="P4" t="n">
-        <v>0.03013953624893626</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -665,99 +665,49 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5861145238282404</v>
+        <v>0.1110330316926266</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4083044997455158</v>
+        <v>0.1072816477638703</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.01246798941549944</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1185400160551497</v>
+        <v>0.3631071155084841</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2035402412591134</v>
+        <v>0.1371478835704938</v>
       </c>
       <c r="H5" t="n">
-        <v>0.02634222579003328</v>
+        <v>0.00825243444337464</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01671006438899598</v>
+        <v>0.01650486888674928</v>
       </c>
       <c r="J5" t="n">
-        <v>0.06585556447508319</v>
+        <v>0.2145632955277406</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6453845318558152</v>
+        <v>0.6106801488097233</v>
       </c>
       <c r="L5" t="n">
-        <v>0.006585556447508319</v>
+        <v>0.03300973777349856</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.01246798941549944</v>
       </c>
       <c r="O5" t="n">
-        <v>0.01975666934252495</v>
+        <v>0.6359164542395885</v>
       </c>
       <c r="P5" t="n">
-        <v>0.1095985914472149</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.9964422428943243</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.08427844668554715</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
+        <v>0.02018782394411392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>